<commit_message>
doing the cm and the layout
</commit_message>
<xml_diff>
--- a/report/logisticreport.xlsx
+++ b/report/logisticreport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Logistic_report_extract\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D376BA36-E716-4734-A36D-0CA9C37F6CB6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6CC520-741C-42DE-BE9F-0F3575310A2E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DDCDFA85-EBA4-44BF-9784-F6ACFB77183C}"/>
+    <workbookView minimized="1" xWindow="7200" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{DDCDFA85-EBA4-44BF-9784-F6ACFB77183C}"/>
   </bookViews>
   <sheets>
     <sheet name="Weekly Report" sheetId="1" r:id="rId1"/>
@@ -1093,7 +1093,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4451727" y="858303"/>
+          <a:off x="5640995" y="814552"/>
           <a:ext cx="330049" cy="152175"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2985,8 +2985,8 @@
   </sheetPr>
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -3124,7 +3124,7 @@
         <v>47</v>
       </c>
       <c r="C5" s="19">
-        <v>12250</v>
+        <v>12230</v>
       </c>
       <c r="D5" s="19" t="s">
         <v>5</v>
@@ -3582,7 +3582,7 @@
       </c>
       <c r="C16" s="6">
         <f>SUM(C5:C15)-C9</f>
-        <v>790695.3</v>
+        <v>790675.3</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="1"/>

</xml_diff>